<commit_message>
Making norm features available.
</commit_message>
<xml_diff>
--- a/data/output/cluster_metrics_dendrogram.xlsx
+++ b/data/output/cluster_metrics_dendrogram.xlsx
@@ -486,11 +486,11 @@
         <v>1.003540763856561</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.004430959909984896</v>
+        <v>0.02502539014123054</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>coldread_gaze_wpm_median</t>
+          <t>norm_coldread_gaze_wpm_median</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -515,11 +515,11 @@
         <v>1.040945115505756</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.04852631801480001</v>
+        <v>0.003128925285112487</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>coldread_saccade_regression_rate_%</t>
+          <t>norm_coldread_saccade_regression_rate_%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -544,11 +544,11 @@
         <v>1.110033313784271</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.05016766550460761</v>
+        <v>0.03959755131507949</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>qa_coverage_line_%</t>
+          <t>norm_qa_coverage_line_%</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">

</xml_diff>

<commit_message>
V1 of the reports.
</commit_message>
<xml_diff>
--- a/data/output/cluster_metrics_dendrogram.xlsx
+++ b/data/output/cluster_metrics_dendrogram.xlsx
@@ -480,13 +480,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6755879905720963</v>
+        <v>0.6752876796897646</v>
       </c>
       <c r="D2" t="n">
-        <v>1.003540763856561</v>
+        <v>1.009167506784137</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02502539014123054</v>
+        <v>0.02204064037765832</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -495,7 +495,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>7.96e-03</t>
+          <t>1.79e-02</t>
         </is>
       </c>
     </row>
@@ -509,22 +509,22 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4875985012353222</v>
+        <v>0.5036067805454411</v>
       </c>
       <c r="D3" t="n">
-        <v>1.040945115505756</v>
+        <v>1.134293978280183</v>
       </c>
       <c r="E3" t="n">
-        <v>0.003128925285112487</v>
+        <v>0.007913767507918164</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>norm_coldread_saccade_regression_rate_%</t>
+          <t>norm_coldread_coverage_line_%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2.10e-01</t>
+          <t>9.00e-02</t>
         </is>
       </c>
     </row>
@@ -535,25 +535,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4898833885006963</v>
+        <v>0.4865644270916379</v>
       </c>
       <c r="D4" t="n">
-        <v>1.110033313784271</v>
+        <v>1.046600125451598</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03959755131507949</v>
+        <v>-0.01688470457019641</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>norm_qa_coverage_line_%</t>
+          <t>norm_coldread_saccade_regression_rate_%</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>3.49e-02</t>
+          <t>3.39e-01</t>
         </is>
       </c>
     </row>

</xml_diff>